<commit_message>
weitere Vitalparameter und englische Version des IGs hinzugefügt
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-t-cabs-diagnosticreport-visitenbefund.xlsx
+++ b/output/StructureDefinition-t-cabs-diagnosticreport-visitenbefund.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="334">
   <si>
     <t>Property</t>
   </si>
@@ -45,7 +45,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>T-CABS DiagnosticReport Visitenbefund</t>
+    <t>T-CABS DiagnosticReport Visit Finding</t>
   </si>
   <si>
     <t>Status</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-16T18:59:10+02:00</t>
+    <t>2025-11-19T11:55:29+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,19 +72,19 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>BIH-CEI (http://example.org/example-publisher)</t>
+    <t>BIH-CEI (https://www.bihealth.org/)</t>
   </si>
   <si>
     <t>Jurisdiction</t>
   </si>
   <si>
-    <t/>
+    <t>Germany</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Profil für einen Beurteilung der wöchentlichen, telemedizinischen Visite innerhalb der T-CABS Studie</t>
+    <t>Profile for an assessment of the weekly telemedicine visit within the T-CABS study</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1577,72 +1580,72 @@
         <v>79</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M2" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N2" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF2" t="s" s="2">
         <v>30</v>
@@ -1654,602 +1657,602 @@
         <v>79</v>
       </c>
       <c r="AI2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ2" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AL2" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AM2" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AN2" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N3" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AG3" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AK3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AN3" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AN4" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N5" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AN5" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N6" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Z6" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AN6" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N7" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM7" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AN7" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
@@ -2259,75 +2262,75 @@
         <v>79</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="N8" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AG8" t="s" s="2">
         <v>78</v>
@@ -2336,34 +2339,34 @@
         <v>79</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM8" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AN8" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
@@ -2373,75 +2376,75 @@
         <v>79</v>
       </c>
       <c r="H9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N9" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>78</v>
@@ -2450,34 +2453,34 @@
         <v>79</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM9" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AN9" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
@@ -2487,77 +2490,77 @@
         <v>79</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O10" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="P10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>78</v>
@@ -2566,34 +2569,34 @@
         <v>79</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM10" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AN10" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s" s="2">
@@ -2603,77 +2606,77 @@
         <v>79</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="N11" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O11" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="P11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>78</v>
@@ -2682,34 +2685,34 @@
         <v>79</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AN11" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s" s="2">
@@ -2719,77 +2722,77 @@
         <v>79</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="O12" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="P12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>78</v>
@@ -2798,148 +2801,148 @@
         <v>79</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AN12" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="Z13" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AA13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s" s="2">
@@ -2949,75 +2952,75 @@
         <v>79</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Z14" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AA14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>78</v>
@@ -3026,608 +3029,608 @@
         <v>79</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S15" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="T15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AA15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="P16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH16" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="P17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH17" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="O18" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="P18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="O19" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="P19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
@@ -3637,77 +3640,77 @@
         <v>79</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="O20" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="P20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>78</v>
@@ -3716,34 +3719,34 @@
         <v>79</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s" s="2">
@@ -3753,77 +3756,77 @@
         <v>79</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="O21" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="P21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>78</v>
@@ -3832,34 +3835,34 @@
         <v>79</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s" s="2">
@@ -3869,77 +3872,77 @@
         <v>79</v>
       </c>
       <c r="H22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="O22" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="P22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>78</v>
@@ -3948,34 +3951,34 @@
         <v>79</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
@@ -3985,77 +3988,77 @@
         <v>79</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="O23" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="P23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>78</v>
@@ -4064,34 +4067,34 @@
         <v>79</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
@@ -4101,75 +4104,75 @@
         <v>79</v>
       </c>
       <c r="H24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>78</v>
@@ -4178,34 +4181,34 @@
         <v>79</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -4215,75 +4218,75 @@
         <v>79</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="P25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>78</v>
@@ -4292,146 +4295,146 @@
         <v>79</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s" s="2">
@@ -4441,75 +4444,75 @@
         <v>79</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>78</v>
@@ -4518,34 +4521,34 @@
         <v>79</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
@@ -4555,77 +4558,77 @@
         <v>79</v>
       </c>
       <c r="H28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I28" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O28" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="P28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>78</v>
@@ -4634,376 +4637,376 @@
         <v>79</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="O29" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="P29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q29" s="2"/>
       <c r="R29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q30" s="2"/>
       <c r="R30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="P31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q31" s="2"/>
       <c r="R31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH31" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
@@ -5013,73 +5016,73 @@
         <v>79</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Z32" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AA32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>78</v>
@@ -5088,34 +5091,34 @@
         <v>79</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
@@ -5125,77 +5128,77 @@
         <v>79</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="O33" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="P33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Q33" s="2"/>
       <c r="R33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="S33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="T33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="U33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="V33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="W33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="X33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="Z33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AA33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AB33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AC33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AD33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>78</v>
@@ -5204,22 +5207,22 @@
         <v>79</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>